<commit_message>
Updates on Data Renames
</commit_message>
<xml_diff>
--- a/Data/income.xlsx
+++ b/Data/income.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BVW/BVW/Harvard/2019-2/Data/Sacred-Profane_04_25_2020/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB07AD5-CF71-BE4B-B51D-AED19BD17C56}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07379FFD-B204-944B-9D4F-97A13BA7CD44}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17800" yWindow="460" windowWidth="15800" windowHeight="19720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -597,9 +597,6 @@
     <t>Lincoln, NE</t>
   </si>
   <si>
-    <t>Little Rock-North Little Rock-Conway, AR</t>
-  </si>
-  <si>
     <t>Logan, UT-ID</t>
   </si>
   <si>
@@ -612,9 +609,6 @@
     <t>Los Angeles-Long Beach-Anaheim, CA</t>
   </si>
   <si>
-    <t>Louisville/Jefferson County, KY-IN</t>
-  </si>
-  <si>
     <t>Lubbock, TX</t>
   </si>
   <si>
@@ -697,9 +691,6 @@
   </si>
   <si>
     <t>Napa, CA</t>
-  </si>
-  <si>
-    <t>Nashville-Davidson--Murfreesboro--Franklin, TN</t>
   </si>
   <si>
     <t>New Bern, NC</t>
@@ -1089,12 +1080,6 @@
     <t>Anniston-Oxford, AL</t>
   </si>
   <si>
-    <t>Atlanta-Sandy Springs-Alpharetta, GA</t>
-  </si>
-  <si>
-    <t>Austin-Round Rock-Georgetown, TX</t>
-  </si>
-  <si>
     <t>Bend, OR</t>
   </si>
   <si>
@@ -1104,30 +1089,12 @@
     <t>Bremerton-Silverdale-Port Orchard, WA</t>
   </si>
   <si>
-    <t>Buffalo-Cheektowaga, NY</t>
-  </si>
-  <si>
-    <t>Dayton-Kettering, OH</t>
-  </si>
-  <si>
     <t>Eugene-Springfield, OR</t>
   </si>
   <si>
-    <t>Fayetteville-Springdale-Rogers, AR</t>
-  </si>
-  <si>
-    <t>Grand Rapids-Kentwood, MI</t>
-  </si>
-  <si>
-    <t>Greenville-Anderson, SC</t>
-  </si>
-  <si>
     <t>Gulfport-Biloxi, MS</t>
   </si>
   <si>
-    <t>Hartford-East Hartford-Middletown, CT</t>
-  </si>
-  <si>
     <t>Hilton Head Island-Bluffton, SC</t>
   </si>
   <si>
@@ -1137,12 +1104,6 @@
     <t>Mankato, MN</t>
   </si>
   <si>
-    <t>Miami-Fort Lauderdale-Pompano Beach, FL</t>
-  </si>
-  <si>
-    <t>Milwaukee-Waukesha, WI</t>
-  </si>
-  <si>
     <t>Naples-Marco Island, FL</t>
   </si>
   <si>
@@ -1152,36 +1113,18 @@
     <t>Olympia-Lacey-Tumwater, WA</t>
   </si>
   <si>
-    <t>Phoenix-Mesa-Chandler, AZ</t>
-  </si>
-  <si>
     <t>Poughkeepsie-Newburgh-Middletown, NY</t>
   </si>
   <si>
     <t>Prescott Valley-Prescott, AZ</t>
   </si>
   <si>
-    <t>Raleigh-Cary, NC</t>
-  </si>
-  <si>
-    <t>Sacramento-Roseville-Folsom, CA</t>
-  </si>
-  <si>
-    <t>San Diego-Chula Vista-Carlsbad, CA</t>
-  </si>
-  <si>
-    <t>San Francisco-Oakland-Berkeley, CA</t>
-  </si>
-  <si>
     <t>San Luis Obispo-Paso Robles, CA</t>
   </si>
   <si>
     <t>Santa Rosa-Petaluma, CA</t>
   </si>
   <si>
-    <t>Scranton--Wilkes-Barre, PA</t>
-  </si>
-  <si>
     <t>Sebring-Avon Park, FL</t>
   </si>
   <si>
@@ -1204,6 +1147,63 @@
   </si>
   <si>
     <t>Enid, OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scranton--Wilkes-Barre--Hazleton, PA	</t>
+  </si>
+  <si>
+    <t>San Diego-Carlsbad, CA</t>
+  </si>
+  <si>
+    <t>San Francisco-Oakland-Hayward, CA</t>
+  </si>
+  <si>
+    <t>Raleigh, NC</t>
+  </si>
+  <si>
+    <t>Phoenix-Mesa-Scottsdale, AZ</t>
+  </si>
+  <si>
+    <t>Nashville-Davidson-Murfreesboro-Franklin, TN</t>
+  </si>
+  <si>
+    <t>Milwaukee-Waukesha-West Allis, WI</t>
+  </si>
+  <si>
+    <t>Miami-Fort Lauderdale-West Palm Beach, FL</t>
+  </si>
+  <si>
+    <t>Louisville-Jefferson County, KY-IN</t>
+  </si>
+  <si>
+    <t>Little Rock-N Little Rock-Conway, AR</t>
+  </si>
+  <si>
+    <t>Hartford-West Hartford-East Hartford, CT</t>
+  </si>
+  <si>
+    <t>Greenville-Anderson-Mauldin, SC</t>
+  </si>
+  <si>
+    <t>Grand Rapids-Wyoming, MI</t>
+  </si>
+  <si>
+    <t>Fayetteville, Springdale-Rogers, AR-MO</t>
+  </si>
+  <si>
+    <t>Dayton, OH</t>
+  </si>
+  <si>
+    <t>Buffalo-Cheektowaga-Niagara Falls, NY</t>
+  </si>
+  <si>
+    <t>Austin-Round Rock, TX</t>
+  </si>
+  <si>
+    <t>Atlanta-Sandy Springs-Roswell, GA</t>
+  </si>
+  <si>
+    <t>Sacramento--Roseville--Arden-Arcade, CA</t>
   </si>
 </sst>
 </file>
@@ -1948,8 +1948,8 @@
   </sheetPr>
   <dimension ref="A1:D390"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A281" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A294" sqref="A294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1960,7 +1960,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B1" s="2">
         <v>2016</v>
@@ -2016,7 +2016,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B5" s="3">
         <v>39164</v>
@@ -2156,7 +2156,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B15" s="3">
         <v>34774</v>
@@ -2212,7 +2212,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
-        <v>349</v>
+        <v>386</v>
       </c>
       <c r="B19" s="3">
         <v>48052</v>
@@ -2268,7 +2268,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
-        <v>350</v>
+        <v>385</v>
       </c>
       <c r="B23" s="3">
         <v>52208</v>
@@ -2422,7 +2422,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B34" s="3">
         <v>50195</v>
@@ -2492,7 +2492,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="B39" s="3">
         <v>35515</v>
@@ -2604,7 +2604,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" s="5" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B47" s="3">
         <v>50518</v>
@@ -2660,7 +2660,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" s="5" t="s">
-        <v>354</v>
+        <v>384</v>
       </c>
       <c r="B51" s="3">
         <v>46327</v>
@@ -3248,7 +3248,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A93" s="5" t="s">
-        <v>355</v>
+        <v>383</v>
       </c>
       <c r="B93" s="3">
         <v>43904</v>
@@ -3514,7 +3514,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A112" s="5" t="s">
-        <v>387</v>
+        <v>368</v>
       </c>
       <c r="B112" s="3">
         <v>43530</v>
@@ -3542,7 +3542,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A114" s="5" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="B114" s="3">
         <v>42254</v>
@@ -3626,7 +3626,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A120" s="5" t="s">
-        <v>357</v>
+        <v>382</v>
       </c>
       <c r="B120" s="3">
         <v>60394</v>
@@ -3892,7 +3892,7 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A139" s="5" t="s">
-        <v>358</v>
+        <v>381</v>
       </c>
       <c r="B139" s="3">
         <v>46966</v>
@@ -3990,7 +3990,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A146" s="5" t="s">
-        <v>359</v>
+        <v>380</v>
       </c>
       <c r="B146" s="3">
         <v>40902</v>
@@ -4004,7 +4004,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A147" s="5" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="B147" s="3">
         <v>35316</v>
@@ -4088,7 +4088,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A153" s="5" t="s">
-        <v>361</v>
+        <v>379</v>
       </c>
       <c r="B153" s="3">
         <v>59902</v>
@@ -4130,7 +4130,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A156" s="5" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="B156" s="3">
         <v>48856</v>
@@ -4536,7 +4536,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A185" s="5" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
       <c r="B185" s="3">
         <v>37138</v>
@@ -4858,7 +4858,7 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A208" s="5" t="s">
-        <v>189</v>
+        <v>378</v>
       </c>
       <c r="B208" s="3">
         <v>42963</v>
@@ -4872,7 +4872,7 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A209" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B209" s="3">
         <v>35406</v>
@@ -4886,7 +4886,7 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A210" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B210" s="3">
         <v>39150</v>
@@ -4900,7 +4900,7 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A211" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B211" s="3">
         <v>41827</v>
@@ -4914,7 +4914,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A212" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B212" s="3">
         <v>58548</v>
@@ -4928,7 +4928,7 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A213" s="5" t="s">
-        <v>194</v>
+        <v>377</v>
       </c>
       <c r="B213" s="3">
         <v>46456</v>
@@ -4942,7 +4942,7 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A214" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B214" s="3">
         <v>39579</v>
@@ -4956,7 +4956,7 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A215" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B215" s="3">
         <v>37598</v>
@@ -4970,7 +4970,7 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A216" s="5" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B216" s="3">
         <v>38120</v>
@@ -4984,7 +4984,7 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A217" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B217" s="3">
         <v>37209</v>
@@ -4998,7 +4998,7 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A218" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B218" s="3">
         <v>54702</v>
@@ -5012,7 +5012,7 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A219" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B219" s="3">
         <v>56615</v>
@@ -5026,7 +5026,7 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A220" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B220" s="3">
         <v>43171</v>
@@ -5040,7 +5040,7 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A221" s="5" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="B221" s="3">
         <v>43513</v>
@@ -5054,7 +5054,7 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A222" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B222" s="3">
         <v>36368</v>
@@ -5068,7 +5068,7 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A223" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B223" s="3">
         <v>25111</v>
@@ -5082,7 +5082,7 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A224" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B224" s="3">
         <v>43151</v>
@@ -5096,7 +5096,7 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A225" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B225" s="3">
         <v>43526</v>
@@ -5110,7 +5110,7 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A226" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B226" s="3">
         <v>36786</v>
@@ -5124,7 +5124,7 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A227" s="5" t="s">
-        <v>365</v>
+        <v>376</v>
       </c>
       <c r="B227" s="3">
         <v>50974</v>
@@ -5138,7 +5138,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A228" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B228" s="3">
         <v>39048</v>
@@ -5152,7 +5152,7 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A229" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B229" s="3">
         <v>47499</v>
@@ -5166,7 +5166,7 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A230" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B230" s="3">
         <v>74624</v>
@@ -5180,7 +5180,7 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A231" s="5" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="B231" s="3">
         <v>52429</v>
@@ -5194,7 +5194,7 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A232" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B232" s="3">
         <v>58345</v>
@@ -5208,7 +5208,7 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A233" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B233" s="3">
         <v>44646</v>
@@ -5222,7 +5222,7 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A234" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B234" s="3">
         <v>35961</v>
@@ -5236,7 +5236,7 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A235" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B235" s="3">
         <v>41417</v>
@@ -5250,7 +5250,7 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A236" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B236" s="3">
         <v>38093</v>
@@ -5264,7 +5264,7 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A237" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B237" s="3">
         <v>43757</v>
@@ -5278,7 +5278,7 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A238" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B238" s="3">
         <v>40608</v>
@@ -5292,7 +5292,7 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A239" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B239" s="3">
         <v>38911</v>
@@ -5306,7 +5306,7 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A240" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B240" s="3">
         <v>33656</v>
@@ -5320,7 +5320,7 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A241" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B241" s="3">
         <v>47870</v>
@@ -5334,7 +5334,7 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A242" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B242" s="3">
         <v>34621</v>
@@ -5348,7 +5348,7 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A243" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B243" s="3">
         <v>36235</v>
@@ -5362,7 +5362,7 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A244" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B244" s="3">
         <v>36563</v>
@@ -5376,7 +5376,7 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A245" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B245" s="3">
         <v>67580</v>
@@ -5390,7 +5390,7 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A246" s="5" t="s">
-        <v>367</v>
+        <v>354</v>
       </c>
       <c r="B246" s="3">
         <v>83659</v>
@@ -5404,7 +5404,7 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A247" s="5" t="s">
-        <v>223</v>
+        <v>374</v>
       </c>
       <c r="B247" s="3">
         <v>53704</v>
@@ -5418,7 +5418,7 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A248" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B248" s="3">
         <v>41019</v>
@@ -5432,7 +5432,7 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A249" s="5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B249" s="3">
         <v>52621</v>
@@ -5446,7 +5446,7 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A250" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B250" s="3">
         <v>48244</v>
@@ -5460,7 +5460,7 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A251" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B251" s="3">
         <v>68512</v>
@@ -5474,7 +5474,7 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A252" s="5" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="B252" s="3">
         <v>44018</v>
@@ -5488,7 +5488,7 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A253" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B253" s="3">
         <v>51775</v>
@@ -5502,7 +5502,7 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A254" s="5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B254" s="3">
         <v>54805</v>
@@ -5516,7 +5516,7 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A255" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B255" s="3">
         <v>34506</v>
@@ -5530,7 +5530,7 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A256" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B256" s="3">
         <v>55995</v>
@@ -5544,7 +5544,7 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A257" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B257" s="3">
         <v>37676</v>
@@ -5558,7 +5558,7 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A258" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B258" s="3">
         <v>40498</v>
@@ -5572,7 +5572,7 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A259" s="5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B259" s="3">
         <v>44460</v>
@@ -5586,7 +5586,7 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A260" s="5" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="B260" s="3">
         <v>47328</v>
@@ -5600,7 +5600,7 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A261" s="5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B261" s="3">
         <v>53285</v>
@@ -5614,7 +5614,7 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A262" s="5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B262" s="3">
         <v>39920</v>
@@ -5628,7 +5628,7 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A263" s="5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B263" s="3">
         <v>44662</v>
@@ -5642,7 +5642,7 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A264" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B264" s="3">
         <v>38753</v>
@@ -5656,7 +5656,7 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A265" s="5" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B265" s="3">
         <v>57136</v>
@@ -5670,7 +5670,7 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A266" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B266" s="3">
         <v>41793</v>
@@ -5684,7 +5684,7 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A267" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B267" s="3">
         <v>41019</v>
@@ -5698,7 +5698,7 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A268" s="5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B268" s="3">
         <v>37757</v>
@@ -5712,7 +5712,7 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A269" s="5" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B269" s="3">
         <v>40315</v>
@@ -5726,7 +5726,7 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A270" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B270" s="3">
         <v>45463</v>
@@ -5740,7 +5740,7 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A271" s="5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B271" s="3">
         <v>60105</v>
@@ -5754,7 +5754,7 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A272" s="5" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="B272" s="3">
         <v>42460</v>
@@ -5768,7 +5768,7 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A273" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B273" s="3">
         <v>32372</v>
@@ -5782,7 +5782,7 @@
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A274" s="5" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B274" s="3">
         <v>51681</v>
@@ -5796,7 +5796,7 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A275" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B275" s="3">
         <v>52595</v>
@@ -5810,7 +5810,7 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A276" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B276" s="3">
         <v>35500</v>
@@ -5824,7 +5824,7 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A277" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B277" s="3">
         <v>52521</v>
@@ -5838,7 +5838,7 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A278" s="5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B278" s="3">
         <v>51683</v>
@@ -5852,7 +5852,7 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A279" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B279" s="3">
         <v>50134</v>
@@ -5866,7 +5866,7 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A280" s="5" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="B280" s="3">
         <v>49419</v>
@@ -5880,7 +5880,7 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A281" s="5" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="B281" s="3">
         <v>36511</v>
@@ -5894,7 +5894,7 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A282" s="5" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B282" s="3">
         <v>50242</v>
@@ -5908,7 +5908,7 @@
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A283" s="5" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B283" s="3">
         <v>37375</v>
@@ -5922,7 +5922,7 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A284" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B284" s="3">
         <v>36228</v>
@@ -5936,7 +5936,7 @@
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A285" s="5" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B285" s="3">
         <v>39292</v>
@@ -5950,7 +5950,7 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A286" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B286" s="3">
         <v>45153</v>
@@ -5964,7 +5964,7 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A287" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B287" s="3">
         <v>51005</v>
@@ -5978,7 +5978,7 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A288" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B288" s="3">
         <v>46692</v>
@@ -5992,7 +5992,7 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A289" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B289" s="3">
         <v>45863</v>
@@ -6006,7 +6006,7 @@
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A290" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B290" s="3">
         <v>43412</v>
@@ -6020,7 +6020,7 @@
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A291" s="5" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B291" s="3">
         <v>52263</v>
@@ -6034,7 +6034,7 @@
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A292" s="5" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B292" s="3">
         <v>53093</v>
@@ -6048,7 +6048,7 @@
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A293" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B293" s="3">
         <v>37774</v>
@@ -6062,7 +6062,7 @@
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A294" s="5" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B294" s="3">
         <v>44292</v>
@@ -6076,7 +6076,7 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A295" s="5" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B295" s="3">
         <v>50068</v>
@@ -6090,7 +6090,7 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A296" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B296" s="3">
         <v>47091</v>
@@ -6104,7 +6104,7 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A297" s="5" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B297" s="3">
         <v>40600</v>
@@ -6118,7 +6118,7 @@
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A298" s="5" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B298" s="3">
         <v>36625</v>
@@ -6132,7 +6132,7 @@
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A299" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B299" s="3">
         <v>36054</v>
@@ -6146,7 +6146,7 @@
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A300" s="5" t="s">
-        <v>374</v>
+        <v>387</v>
       </c>
       <c r="B300" s="3">
         <v>52436</v>
@@ -6160,7 +6160,7 @@
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A301" s="5" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B301" s="3">
         <v>36722</v>
@@ -6174,7 +6174,7 @@
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A302" s="5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B302" s="3">
         <v>42971</v>
@@ -6188,7 +6188,7 @@
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A303" s="5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B303" s="3">
         <v>34775</v>
@@ -6202,7 +6202,7 @@
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A304" s="5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B304" s="3">
         <v>36629</v>
@@ -6216,7 +6216,7 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A305" s="5" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B305" s="3">
         <v>51500</v>
@@ -6230,7 +6230,7 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A306" s="5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B306" s="3">
         <v>39529</v>
@@ -6244,7 +6244,7 @@
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A307" s="5" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B307" s="3">
         <v>52686</v>
@@ -6258,7 +6258,7 @@
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A308" s="5" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B308" s="3">
         <v>45466</v>
@@ -6272,7 +6272,7 @@
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A309" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B309" s="3">
         <v>47394</v>
@@ -6286,7 +6286,7 @@
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A310" s="5" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B310" s="3">
         <v>41962</v>
@@ -6300,7 +6300,7 @@
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A311" s="5" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B311" s="3">
         <v>43324</v>
@@ -6314,7 +6314,7 @@
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A312" s="5" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="B312" s="3">
         <v>56322</v>
@@ -6328,7 +6328,7 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A313" s="5" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B313" s="3">
         <v>86852</v>
@@ -6342,7 +6342,7 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A314" s="5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B314" s="3">
         <v>91198</v>
@@ -6356,7 +6356,7 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A315" s="5" t="s">
-        <v>377</v>
+        <v>359</v>
       </c>
       <c r="B315" s="3">
         <v>53041</v>
@@ -6370,7 +6370,7 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A316" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B316" s="3">
         <v>61166</v>
@@ -6384,7 +6384,7 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A317" s="5" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B317" s="3">
         <v>54386</v>
@@ -6398,7 +6398,7 @@
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A318" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B318" s="3">
         <v>57432</v>
@@ -6412,7 +6412,7 @@
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A319" s="5" t="s">
-        <v>378</v>
+        <v>360</v>
       </c>
       <c r="B319" s="3">
         <v>57566</v>
@@ -6426,7 +6426,7 @@
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A320" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B320" s="3">
         <v>43177</v>
@@ -6440,7 +6440,7 @@
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A321" s="5" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="B321" s="3">
         <v>42721</v>
@@ -6454,7 +6454,7 @@
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A322" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B322" s="3">
         <v>66358</v>
@@ -6468,7 +6468,7 @@
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A323" s="5" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B323" s="3">
         <v>69832</v>
@@ -6482,7 +6482,7 @@
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A324" s="5" t="s">
-        <v>380</v>
+        <v>361</v>
       </c>
       <c r="B324" s="3">
         <v>32174</v>
@@ -6496,7 +6496,7 @@
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A325" s="5" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B325" s="3">
         <v>47936</v>
@@ -6510,7 +6510,7 @@
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A326" s="5" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B326" s="3">
         <v>39971</v>
@@ -6524,7 +6524,7 @@
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A327" s="5" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B327" s="3">
         <v>43350</v>
@@ -6538,7 +6538,7 @@
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A328" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B328" s="3">
         <v>37621</v>
@@ -6552,7 +6552,7 @@
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A329" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B329" s="3">
         <v>47174</v>
@@ -6566,7 +6566,7 @@
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A330" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B330" s="3">
         <v>56085</v>
@@ -6580,7 +6580,7 @@
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A331" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B331" s="3">
         <v>43477</v>
@@ -6594,7 +6594,7 @@
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A332" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B332" s="3">
         <v>40785</v>
@@ -6608,7 +6608,7 @@
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A333" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B333" s="3">
         <v>42397</v>
@@ -6622,7 +6622,7 @@
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A334" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B334" s="3">
         <v>44680</v>
@@ -6636,7 +6636,7 @@
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A335" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B335" s="3">
         <v>48770</v>
@@ -6650,7 +6650,7 @@
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A336" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B336" s="3">
         <v>38464</v>
@@ -6664,7 +6664,7 @@
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A337" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B337" s="3">
         <v>37843</v>
@@ -6678,7 +6678,7 @@
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A338" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B338" s="3">
         <v>42183</v>
@@ -6692,7 +6692,7 @@
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A339" s="5" t="s">
-        <v>381</v>
+        <v>362</v>
       </c>
       <c r="B339" s="3">
         <v>41224</v>
@@ -6706,7 +6706,7 @@
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A340" s="5" t="s">
-        <v>382</v>
+        <v>363</v>
       </c>
       <c r="B340" s="3">
         <v>41094</v>
@@ -6720,7 +6720,7 @@
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A341" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B341" s="3">
         <v>34573</v>
@@ -6734,7 +6734,7 @@
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A342" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B342" s="3">
         <v>45393</v>
@@ -6748,7 +6748,7 @@
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A343" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B343" s="3">
         <v>39419</v>
@@ -6762,7 +6762,7 @@
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A344" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B344" s="3">
         <v>43763</v>
@@ -6776,7 +6776,7 @@
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A345" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B345" s="3">
         <v>35425</v>
@@ -6790,7 +6790,7 @@
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A346" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B346" s="3">
         <v>35637</v>
@@ -6804,7 +6804,7 @@
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A347" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B347" s="3">
         <v>42126</v>
@@ -6818,7 +6818,7 @@
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A348" s="5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B348" s="3">
         <v>43742</v>
@@ -6832,7 +6832,7 @@
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A349" s="5" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B349" s="3">
         <v>42951</v>
@@ -6846,7 +6846,7 @@
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A350" s="5" t="s">
-        <v>383</v>
+        <v>364</v>
       </c>
       <c r="B350" s="3">
         <v>64505</v>
@@ -6860,7 +6860,7 @@
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A351" s="5" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B351" s="3">
         <v>39904</v>
@@ -6874,7 +6874,7 @@
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A352" s="5" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B352" s="3">
         <v>48035</v>
@@ -6888,7 +6888,7 @@
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A353" s="5" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B353" s="3">
         <v>35421</v>
@@ -6902,7 +6902,7 @@
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A354" s="5" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B354" s="3">
         <v>36994</v>
@@ -6916,7 +6916,7 @@
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A355" s="5" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B355" s="3">
         <v>46218</v>
@@ -6930,7 +6930,7 @@
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A356" s="5" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B356" s="3">
         <v>54860</v>
@@ -6944,7 +6944,7 @@
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A357" s="5" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B357" s="3">
         <v>40418</v>
@@ -6958,7 +6958,7 @@
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A358" s="5" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B358" s="3">
         <v>33664</v>
@@ -6972,7 +6972,7 @@
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A359" s="5" t="s">
-        <v>384</v>
+        <v>365</v>
       </c>
       <c r="B359" s="3">
         <v>46999</v>
@@ -6986,7 +6986,7 @@
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A360" s="5" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B360" s="3">
         <v>41507</v>
@@ -7000,7 +7000,7 @@
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A361" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B361" s="3">
         <v>37515</v>
@@ -7014,7 +7014,7 @@
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A362" s="5" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B362" s="3">
         <v>46992</v>
@@ -7028,7 +7028,7 @@
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A363" s="5" t="s">
-        <v>385</v>
+        <v>366</v>
       </c>
       <c r="B363" s="3">
         <v>38198</v>
@@ -7042,7 +7042,7 @@
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A364" s="5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B364" s="3">
         <v>37897</v>
@@ -7056,7 +7056,7 @@
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A365" s="5" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B365" s="3">
         <v>42464</v>
@@ -7070,7 +7070,7 @@
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A366" s="5" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B366" s="3">
         <v>39342</v>
@@ -7084,7 +7084,7 @@
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A367" s="5" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B367" s="3">
         <v>67795</v>
@@ -7098,7 +7098,7 @@
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A368" s="5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B368" s="3">
         <v>42227</v>
@@ -7112,7 +7112,7 @@
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A369" s="5" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B369" s="3">
         <v>43674</v>
@@ -7126,7 +7126,7 @@
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A370" s="5" t="s">
-        <v>386</v>
+        <v>367</v>
       </c>
       <c r="B370" s="3">
         <v>45753</v>
@@ -7140,7 +7140,7 @@
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A371" s="5" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B371" s="3">
         <v>36579</v>
@@ -7154,7 +7154,7 @@
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A372" s="5" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B372" s="3">
         <v>45838</v>
@@ -7168,7 +7168,7 @@
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A373" s="5" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B373" s="3">
         <v>41229</v>
@@ -7182,7 +7182,7 @@
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A374" s="5" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B374" s="3">
         <v>46659</v>
@@ -7196,7 +7196,7 @@
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A375" s="5" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B375" s="3">
         <v>40194</v>
@@ -7210,7 +7210,7 @@
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A376" s="5" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B376" s="3">
         <v>39990</v>
@@ -7224,7 +7224,7 @@
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A377" s="5" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B377" s="3">
         <v>41122</v>
@@ -7238,7 +7238,7 @@
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A378" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B378" s="3">
         <v>44857</v>
@@ -7252,7 +7252,7 @@
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A379" s="5" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B379" s="3">
         <v>41559</v>
@@ -7266,7 +7266,7 @@
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A380" s="5" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B380" s="3">
         <v>51762</v>
@@ -7280,7 +7280,7 @@
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A381" s="5" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B381" s="3">
         <v>40285</v>
@@ -7294,7 +7294,7 @@
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A382" s="5" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B382" s="3">
         <v>45971</v>
@@ -7308,7 +7308,7 @@
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A383" s="5" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B383" s="3">
         <v>39440</v>
@@ -7322,7 +7322,7 @@
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A384" s="5" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B384" s="3">
         <v>40729</v>
@@ -7336,7 +7336,7 @@
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A385" s="5" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B385" s="3">
         <v>33141</v>
@@ -7350,7 +7350,7 @@
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A386" s="7" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B386" s="8"/>
       <c r="C386" s="8"/>
@@ -7358,7 +7358,7 @@
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A387" s="7" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B387" s="8"/>
       <c r="C387" s="8"/>

</xml_diff>